<commit_message>
feat: add print settings
</commit_message>
<xml_diff>
--- a/test/expected/print.xlsx
+++ b/test/expected/print.xlsx
@@ -11,6 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$11</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$B,Sheet1!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -374,5 +375,9 @@
   <printOptions horizontalCentered="1" verticalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="110" orientation="landscape" blackAndWhite="1" draft="1" horizontalDpi="200" verticalDpi="200"/>
+  <headerFooter>
+    <oddHeader>&amp;CHello</oddHeader>
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add print settings (#73)
</commit_message>
<xml_diff>
--- a/test/expected/print.xlsx
+++ b/test/expected/print.xlsx
@@ -11,6 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$11</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$B,Sheet1!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -374,5 +375,9 @@
   <printOptions horizontalCentered="1" verticalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="110" orientation="landscape" blackAndWhite="1" draft="1" horizontalDpi="200" verticalDpi="200"/>
+  <headerFooter>
+    <oddHeader>&amp;CHello</oddHeader>
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: fix test setHeader, setFooter
</commit_message>
<xml_diff>
--- a/test/expected/print.xlsx
+++ b/test/expected/print.xlsx
@@ -376,8 +376,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="110" orientation="landscape" blackAndWhite="1" draft="1" horizontalDpi="200" verticalDpi="200"/>
   <headerFooter>
-    <oddHeader>&amp;CHello</oddHeader>
-    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
+    <oddFooter>&amp;C&amp;G&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <legacyDrawingHF r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add set_header_image, set_footer_image (#93)
* feat: add set_header_image, set_footer_image

* chore: fix test setHeader, setFooter
</commit_message>
<xml_diff>
--- a/test/expected/print.xlsx
+++ b/test/expected/print.xlsx
@@ -376,8 +376,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="110" orientation="landscape" blackAndWhite="1" draft="1" horizontalDpi="200" verticalDpi="200"/>
   <headerFooter>
-    <oddHeader>&amp;CHello</oddHeader>
-    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
+    <oddFooter>&amp;C&amp;G&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <legacyDrawingHF r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>